<commit_message>
update bien ban tuan 3 va 4
</commit_message>
<xml_diff>
--- a/KeHoachLamViecNhom8.xlsx
+++ b/KeHoachLamViecNhom8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DACN\DACN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C5CB8D-CE10-48D6-9193-BB3F77915605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5AA186-DD23-476C-B6FB-4DC44E101FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C181D8B-8276-4055-B352-AFFEDF803FEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Kế hoạch làm việc nhóm</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Tổng hợp và viết báo cáo chương 3</t>
   </si>
   <si>
-    <t>Nhóm: 19</t>
-  </si>
-  <si>
     <t>Xác định usecase và mối quan hệ giữa các use case</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Thành viên nhóm - Team members:Trần Công Đại Dương,Nguyễn Xuân Dương,Hoàng Quý Dương,Giàng Tùng Dương</t>
+  </si>
+  <si>
+    <t>Nhóm: 8</t>
   </si>
 </sst>
 </file>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292127A4-2DAE-4E05-BF4A-D06A73607139}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +646,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -736,7 +736,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -764,7 +764,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -953,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8">
         <v>45563</v>
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="11">
         <v>45564</v>
@@ -1043,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="11">
         <v>45564</v>
@@ -1057,9 +1057,15 @@
       <c r="F12" s="11">
         <v>45565</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1082,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="11">
         <v>45573</v>
@@ -1122,7 +1128,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="11">
         <v>45579</v>
@@ -1202,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="11">
         <v>45588</v>
@@ -1242,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="13">
         <v>45592</v>
@@ -1282,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="13">
         <v>45600</v>
@@ -1322,7 +1328,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="13">
         <v>45614</v>
@@ -1362,7 +1368,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="13">
         <v>45626</v>

</xml_diff>